<commit_message>
update new GIT commands
</commit_message>
<xml_diff>
--- a/Training.xlsx
+++ b/Training.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandbox\practicas\practicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5AECA4-064A-408E-B775-A8F8EB458E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224C7859-C4E2-4BC4-B388-85027B94351C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GIT" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Git</t>
   </si>
@@ -123,13 +123,49 @@
   </si>
   <si>
     <t>SonarQ | Fortify</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>para conocer la rama en la que estamos</t>
+  </si>
+  <si>
+    <t>git branch [nombre_nueva_rama]</t>
+  </si>
+  <si>
+    <t>crea nueva rama. (pero no nos ubica en la nueva rama creada)</t>
+  </si>
+  <si>
+    <t>git show-branch</t>
+  </si>
+  <si>
+    <t>conocer el detalle de las ramas</t>
+  </si>
+  <si>
+    <t>git checkout [rama_que_queremos_sea_la_activa]</t>
+  </si>
+  <si>
+    <t>permite crear la rama y moverte a ella (hacerla activa) con un solo comando</t>
+  </si>
+  <si>
+    <t>incorporar al master. IMPORTANTE: se debe estar ubicado en la rama master (git checkout master) para fusionar con cualquier rama que queramos</t>
+  </si>
+  <si>
+    <t>git merge master -m "Esto es un merge de master en el brach activo"</t>
+  </si>
+  <si>
+    <t>[nota: origin es el nombre que se suele dar al repositorio remoto]</t>
+  </si>
+  <si>
+    <t>Publica una rama en el repositorio remoto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +183,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -192,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -215,6 +259,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -496,58 +541,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>7</v>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -555,6 +651,7 @@
     <hyperlink ref="A1" r:id="rId1" xr:uid="{8E96DF96-46A3-44FF-A080-4C2BD3FBC8E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -562,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53589ED5-17BB-421C-9A07-999CC390C5CF}">
   <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>

</xml_diff>